<commit_message>
mapping and EA updated
</commit_message>
<xml_diff>
--- a/02-Vocabularies/RPaM/MS-RPaM/RPaM-mapping to MS-dataModels-v1.1.xlsx
+++ b/02-Vocabularies/RPaM/MS-RPaM/RPaM-mapping to MS-dataModels-v1.1.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="313">
   <si>
     <t>This spread-sheet details the content of different MS eMandates and maps it to the RPaM Conceptual Data Model</t>
   </si>
@@ -768,9 +768,6 @@
     <t>xs:unsignedLong</t>
   </si>
   <si>
-    <t>xs:string</t>
-  </si>
-  <si>
     <t>ConsultarApoderamientosResponse/ListaApoderamientos/DatosApoderamientoType/CodApoderamientoINT</t>
   </si>
   <si>
@@ -817,6 +814,162 @@
   </si>
   <si>
     <t>xs:string [200]</t>
+  </si>
+  <si>
+    <t>ConsultarApoderamientosResponse/ListaApoderamientos/DatosApoderamientoType/DatosPordedante/PersonaFisica/IdentificacionPF</t>
+  </si>
+  <si>
+    <t>ConsultarApoderamientosResponse/ListaApoderamientos/DatosApoderamientoType/DatosPordedante/PersonaFisica/Nombre</t>
+  </si>
+  <si>
+    <t>ConsultarApoderamientosResponse/ListaApoderamientos/DatosApoderamientoType/DatosPordedante/PersonaFisica/Apellido1</t>
+  </si>
+  <si>
+    <t>ConsultarApoderamientosResponse/ListaApoderamientos/DatosApoderamientoType/DatosPordedante/PersonaFisica/Apellido2</t>
+  </si>
+  <si>
+    <t>ConsultarApoderamientosResponse/ListaApoderamientos/DatosApoderamientoType/DatosPordedante/PersonaFisica/Email</t>
+  </si>
+  <si>
+    <t>ConsultarApoderamientosResponse/ListaApoderamientos/DatosApoderamientoType/DatosPordedante/PersonaFisica/Telefono</t>
+  </si>
+  <si>
+    <t>ConsultarApoderamientosResponse/ListaApoderamientos/DatosApoderamientoType/DatosPordedante/PersonaFisica/Domicilio</t>
+  </si>
+  <si>
+    <t>ConsultarApoderamientosResponse/ListaApoderamientos/DatosApoderamientoType/DatosPordedante/PersonaJuridica/IdentificacionPJ</t>
+  </si>
+  <si>
+    <t>ConsultarApoderamientosResponse/ListaApoderamientos/DatosApoderamientoType/DatosPordedante/PersonaJuridica/RazonSocial</t>
+  </si>
+  <si>
+    <t>ConsultarApoderamientosResponse/ListaApoderamientos/DatosApoderamientoType/DatosPordedante/PersonaJuridica/Email</t>
+  </si>
+  <si>
+    <t>ConsultarApoderamientosResponse/ListaApoderamientos/DatosApoderamientoType/DatosPordedante/PersonaJuridica/Telefono</t>
+  </si>
+  <si>
+    <t>ConsultarApoderamientosResponse/ListaApoderamientos/DatosApoderamientoType/DatosPordedante/PersonaJuridica/Domicilio</t>
+  </si>
+  <si>
+    <t>ConsultarApoderamientosResponse/ListaApoderamientos/DatosApoderamientoType/DatosPordedante/Representante</t>
+  </si>
+  <si>
+    <t>ConsultarApoderamientosResponse/ListaApoderamientos/DatosApoderamientoType/DatosApoderado/Representante</t>
+  </si>
+  <si>
+    <t>ConsultarApoderamientosResponse/ListaApoderamientos/ListaAnexos</t>
+  </si>
+  <si>
+    <t>ConsultarApoderamientosResponse/ListaApoderamientos/ListaAnexos/NombreDocumento</t>
+  </si>
+  <si>
+    <t>ConsultarApoderamientosResponse/ListaApoderamientos/ListaAnexos/TipoDocumento</t>
+  </si>
+  <si>
+    <t>ConsultarApoderamientosResponse/ListaApoderamientos/ListaAnexos/CSV</t>
+  </si>
+  <si>
+    <t>Secure document verification code</t>
+  </si>
+  <si>
+    <t>Type of anex's document</t>
+  </si>
+  <si>
+    <t>Name of the anex's document</t>
+  </si>
+  <si>
+    <t>xs:string [2]</t>
+  </si>
+  <si>
+    <t>Period of validity of the mandate.</t>
+  </si>
+  <si>
+    <t>Current status of the mandate.</t>
+  </si>
+  <si>
+    <t>Mandate Type.</t>
+  </si>
+  <si>
+    <t>Identificador único de apoderamiento en REA externo.</t>
+  </si>
+  <si>
+    <t>Identificador único de apoderamiento en el REA del MINHAP.</t>
+  </si>
+  <si>
+    <t>Information about the mandator.</t>
+  </si>
+  <si>
+    <t>Information about the mandatee.</t>
+  </si>
+  <si>
+    <t>Information list of the annexes associated with the mandate.</t>
+  </si>
+  <si>
+    <t>Information about the natural person.</t>
+  </si>
+  <si>
+    <t>Information about the legal person.</t>
+  </si>
+  <si>
+    <t>First surname of the NP</t>
+  </si>
+  <si>
+    <t>Firsrt name of the NP</t>
+  </si>
+  <si>
+    <t>Second surname of the NP</t>
+  </si>
+  <si>
+    <t>email address of the NP</t>
+  </si>
+  <si>
+    <t>Phone number of the NP</t>
+  </si>
+  <si>
+    <t>Postal address of the NP</t>
+  </si>
+  <si>
+    <t>NIF or NIE of the NP</t>
+  </si>
+  <si>
+    <t>Official name of the LP</t>
+  </si>
+  <si>
+    <t>email address of the LP</t>
+  </si>
+  <si>
+    <t>Phone number of the LP</t>
+  </si>
+  <si>
+    <t>Postal address of the LP</t>
+  </si>
+  <si>
+    <t>Error type code</t>
+  </si>
+  <si>
+    <t>Information of the error of the LP</t>
+  </si>
+  <si>
+    <t>Xs:string [40]</t>
+  </si>
+  <si>
+    <t>xs:string [100]</t>
+  </si>
+  <si>
+    <t>xs:string [20]</t>
+  </si>
+  <si>
+    <t>xs:string [50]</t>
+  </si>
+  <si>
+    <t>CIF entity number with or without legal personality.</t>
+  </si>
+  <si>
+    <t>xs:string [10]</t>
+  </si>
+  <si>
+    <t>xs:string [9]</t>
   </si>
 </sst>
 </file>
@@ -901,7 +1054,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1041,12 +1194,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1173,6 +1357,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2034,10 +2225,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:O34"/>
+  <dimension ref="B3:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2046,7 +2237,7 @@
     <col min="2" max="2" width="5.7109375" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="101.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -2054,7 +2245,7 @@
     <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20.85546875" customWidth="1"/>
-    <col min="15" max="15" width="21.42578125" customWidth="1"/>
+    <col min="15" max="15" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
@@ -2649,135 +2840,771 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="17"/>
-      <c r="C20" s="18" t="s">
+    <row r="20" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="12"/>
+      <c r="C20" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19" t="s">
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="I20" s="17" t="s">
+      <c r="I20" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="J20" s="18" t="s">
+      <c r="J20" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="K20" s="18" t="s">
+      <c r="K20" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="L20" s="18" t="s">
+      <c r="L20" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="M20" s="19" t="s">
+      <c r="M20" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="N20" s="18"/>
-      <c r="O20" s="20" t="s">
+      <c r="N20" s="13"/>
+      <c r="O20" s="16" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C21" s="21" t="s">
+      <c r="B21" s="64"/>
+      <c r="C21" s="65" t="s">
         <v>242</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="D21" s="65" t="s">
+        <v>245</v>
+      </c>
+      <c r="E21" s="66" t="s">
+        <v>287</v>
+      </c>
+      <c r="F21" s="66" t="s">
+        <v>244</v>
+      </c>
+      <c r="G21" s="66"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="66"/>
+      <c r="J21" s="66"/>
+      <c r="K21" s="66"/>
+      <c r="L21" s="66"/>
+      <c r="M21" s="66"/>
+      <c r="N21" s="66"/>
+      <c r="O21" s="68"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="12"/>
+      <c r="C22" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D22" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="E21" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="E22" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="F22" s="13" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D22" s="21" t="s">
+      <c r="G22" s="13"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="15"/>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23" s="12"/>
+      <c r="C23" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D23" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="E22" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D23" s="21" t="s">
+      <c r="E23" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="15"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="12"/>
+      <c r="C24" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D24" s="21" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D24" s="21" t="s">
+      <c r="E24" s="21" t="s">
+        <v>284</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="G24" s="13"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="15"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B25" s="12"/>
+      <c r="C25" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D25" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="F24" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D25" s="21" t="s">
+      <c r="E25" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="15"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B26" s="12"/>
+      <c r="C26" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D26" s="21" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D26" s="21" t="s">
+      <c r="E26" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="15"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B27" s="12"/>
+      <c r="C27" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D27" s="21" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D27" s="21" t="s">
+      <c r="E27" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="15"/>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B28" s="12"/>
+      <c r="C28" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="G28" s="13"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="15"/>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="12"/>
+      <c r="C29" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>262</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="G29" s="13"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="15"/>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B30" s="12"/>
+      <c r="C30" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>263</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>293</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="G30" s="13"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="15"/>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B31" s="12"/>
+      <c r="C31" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>295</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="G31" s="13"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="15"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B32" s="12"/>
+      <c r="C32" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>296</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="G32" s="13"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="15"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B33" s="12"/>
+      <c r="C33" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>297</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="G33" s="13"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="15"/>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B34" s="12"/>
+      <c r="C34" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>298</v>
+      </c>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="15"/>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B35" s="12"/>
+      <c r="C35" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D35" s="21" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D28" s="21" t="s">
+      <c r="E35" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+      <c r="O35" s="15"/>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B36" s="12"/>
+      <c r="C36" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="G36" s="13"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="15"/>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B37" s="12"/>
+      <c r="C37" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>300</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="G37" s="13"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="15"/>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B38" s="12"/>
+      <c r="C38" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="G38" s="13"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="15"/>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B39" s="12"/>
+      <c r="C39" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D39" s="21" t="s">
+        <v>271</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>302</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="G39" s="13"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
+      <c r="N39" s="13"/>
+      <c r="O39" s="15"/>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B40" s="12"/>
+      <c r="C40" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D40" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="E40" s="21" t="s">
+        <v>303</v>
+      </c>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+      <c r="N40" s="13"/>
+      <c r="O40" s="15"/>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B41" s="12"/>
+      <c r="C41" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>273</v>
+      </c>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="13"/>
+      <c r="O41" s="15"/>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B42" s="12"/>
+      <c r="C42" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D42" s="21" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D29" s="21" t="s">
+      <c r="E42" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
+      <c r="N42" s="13"/>
+      <c r="O42" s="15"/>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B43" s="12"/>
+      <c r="C43" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D43" s="21" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D30" s="21" t="s">
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="15"/>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B44" s="12"/>
+      <c r="C44" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D44" s="21" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D31" s="21" t="s">
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
+      <c r="M44" s="13"/>
+      <c r="N44" s="13"/>
+      <c r="O44" s="15"/>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B45" s="12"/>
+      <c r="C45" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>274</v>
+      </c>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="13"/>
+      <c r="N45" s="13"/>
+      <c r="O45" s="15"/>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B46" s="12"/>
+      <c r="C46" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>275</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="13"/>
+      <c r="N46" s="13"/>
+      <c r="O46" s="15"/>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B47" s="12"/>
+      <c r="C47" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D47" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="F47" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="G47" s="13"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
+      <c r="M47" s="13"/>
+      <c r="N47" s="13"/>
+      <c r="O47" s="15"/>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B48" s="12"/>
+      <c r="C48" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D48" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="G48" s="13"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="13"/>
+      <c r="M48" s="13"/>
+      <c r="N48" s="13"/>
+      <c r="O48" s="15"/>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B49" s="12"/>
+      <c r="C49" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>278</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="F49" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="G49" s="13"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="13"/>
+      <c r="N49" s="13"/>
+      <c r="O49" s="15"/>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B50" s="12"/>
+      <c r="C50" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D50" s="13" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="13"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13"/>
+      <c r="M50" s="13"/>
+      <c r="N50" s="13"/>
+      <c r="O50" s="15"/>
+    </row>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B51" s="12"/>
+      <c r="C51" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D51" s="13" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
+      <c r="E51" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="F51" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="G51" s="13"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13"/>
+      <c r="L51" s="13"/>
+      <c r="M51" s="13"/>
+      <c r="N51" s="13"/>
+      <c r="O51" s="15"/>
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B52" s="17"/>
+      <c r="C52" s="30" t="s">
+        <v>242</v>
+      </c>
+      <c r="D52" s="18" t="s">
         <v>258</v>
       </c>
-      <c r="F33" t="s">
+      <c r="E52" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="F52" s="18" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
-        <v>259</v>
-      </c>
-      <c r="F34" t="s">
-        <v>261</v>
-      </c>
+      <c r="G52" s="18"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="18"/>
+      <c r="J52" s="18"/>
+      <c r="K52" s="18"/>
+      <c r="L52" s="18"/>
+      <c r="M52" s="18"/>
+      <c r="N52" s="18"/>
+      <c r="O52" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>